<commit_message>
fixed typo in class name
fixed typo in class  name
</commit_message>
<xml_diff>
--- a/src/main/resources/vpd/20200624/VPD_20200624.xlsx
+++ b/src/main/resources/vpd/20200624/VPD_20200624.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crosin\OneDrive - National Institute of Standards and Technology (NIST)\ELR APHL\VPD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\elr-aphl-r1-message-validation\src\main\resources\vpd\20200624\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{EDA41962-49E2-4299-9972-695AC10F4C02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{1A8F0A9C-EF28-4597-92F9-9BBCA90129D7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204ADCCD-365F-4EED-A229-3BE7CC6F3FE2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="2520" windowWidth="27390" windowHeight="15480" tabRatio="722" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1920" windowWidth="27390" windowHeight="15480" tabRatio="722" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="5" r:id="rId1"/>
@@ -2198,7 +2198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C525"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A488" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
@@ -7995,9 +7995,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>